<commit_message>
updated waste model + TCH_PWR, TCH_IND and TCH_COM pre TCH_TRA imp files
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/hdri for satim june2020.xlsx
+++ b/SATIM/DataSpreadsheets/hdri for satim june2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryce\Google Drive\Work\Projects Current\SA NDC 2020 shared folder\A.3.- Model update &amp; Calibration\Model stuff\SATIM files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E55303-0905-4F63-94AC-375EF19C2C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885D8F18-4E06-43BC-9746-A0499893BA59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{AC7EF963-3D10-42A6-8D34-6AEAF2076509}"/>
+    <workbookView xWindow="585" yWindow="570" windowWidth="27555" windowHeight="13575" activeTab="5" xr2:uid="{AC7EF963-3D10-42A6-8D34-6AEAF2076509}"/>
   </bookViews>
   <sheets>
     <sheet name="RegionInfo" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,13 +427,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -445,13 +457,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -888,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E832A3-E411-4319-95FC-5A033716DE80}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D27AD4-49AC-41AC-94AE-26BF9DF0D607}">
   <dimension ref="A1:AP42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2:AN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,45 +1464,6 @@
       <c r="R2">
         <v>0</v>
       </c>
-      <c r="AB2">
-        <v>1</v>
-      </c>
-      <c r="AC2">
-        <v>1.3</v>
-      </c>
-      <c r="AD2">
-        <v>1.6</v>
-      </c>
-      <c r="AE2">
-        <v>1.9</v>
-      </c>
-      <c r="AF2">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="AG2">
-        <v>2.5</v>
-      </c>
-      <c r="AH2">
-        <v>2.8</v>
-      </c>
-      <c r="AI2">
-        <v>3.1</v>
-      </c>
-      <c r="AJ2">
-        <v>3.4</v>
-      </c>
-      <c r="AK2">
-        <v>3.7</v>
-      </c>
-      <c r="AL2">
-        <v>4</v>
-      </c>
-      <c r="AM2">
-        <v>5.5</v>
-      </c>
-      <c r="AN2">
-        <v>7</v>
-      </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -3246,8 +3222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64497EF-7933-4B50-839A-5B2954D1C8D5}">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3992,8 +3968,8 @@
       <c r="H29" t="s">
         <v>85</v>
       </c>
-      <c r="I29">
-        <v>2029</v>
+      <c r="I29" s="1">
+        <v>2040</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>